<commit_message>
Analysis + Processing Added
</commit_message>
<xml_diff>
--- a/RB_LLM_results.xlsx
+++ b/RB_LLM_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\MSc Thesis\MSc Code\github\MSc_Thesis_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AD463D-7709-4D95-8E6B-DCB46BFFE40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE5C53C-E46C-4A8D-9987-B7384EE209A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="635">
   <si>
     <t>DateTime</t>
   </si>
@@ -1929,6 +1929,15 @@
   </si>
   <si>
     <t>llm</t>
+  </si>
+  <si>
+    <t>20250421_112414</t>
+  </si>
+  <si>
+    <t>[{'role': 'assistant', 'content': "Hi! I'm excited to start our negotiation. As we begin, I'd like to get a sense of your needs and constraints. Can you share with me your Base Production Cost?"}, {'role': 'user', 'content': "I'm glad you're enthusiastic about the negotiation! My Base Production Cost is €3 per unit, and I must emphasize that this is my absolute minimum cost. Any production cost above this would significantly impact my profit margins.\n\nNow, let's focus on finding a mutually beneficial agreement. As the Supplier, I'm looking to negotiate a quality level that will ensure I maintain a decent profit while still meeting your needs as the Buyer."}, {'role': 'assistant', 'content': 'Confirming: Is 3 the correct Base Production Cost (PC)?\nIf it is correct, please ONLY return 3 again in the chat.\nOtherwise return your current Base Production Cost (PC) at the quality level of 0.\n'}, {'role': 'user', 'content': '3'}, {'role': 'assistant', 'content': 'Thanks, for confirming this information with me.\nWhat combination of Price and Quality do you have in mind to sell me a 10kg pellet bag? Please return the current proposal in square brackets. For example [Wholesale Price, Quality].'}, {'role': 'user', 'content': "Based on my negotiation strategy, I'm proposing [High, Low] for the wholesale price and quality respectively. This combination aligns with my goal of maximizing profits while meeting your needs as a buyer."}, {'role': 'assistant', 'content': 'I am sorry, but your offer is not valid. This is either because I did not recognize it, proposed terms were out of bounds or price or quality were not integers. How about Wholesale Price of 9€ and quality of 4? If you are not satisfied with this offer, please return  your counter proposal in square brackets. For example [Wholesale Price, Quality]. Only put integers in the squared brackets. '}, {'role': 'user', 'content': "I apologize for the confusion earlier! Since my goal is to maximize profits while meeting your needs as a buyer, I'm proposing [6, 0] as a counteroffer. This combination aligns with my negotiation strategy and takes into account our discussion on base production costs."}, {'role': 'assistant', 'content': 'I am pleased to accept your offer! Thank you for investing time and effort in these negotiations! I look forward to a successful partnership.'}]</t>
+  </si>
+  <si>
+    <t>[{'idx': 1745227431, 'price': None, 'quality': None, 'offer_by': 'supplier', 'stamp': 1745227431, 'from_chat': True, 'enhanced': None, 'profit_bot1': -10, 'profit_bot2': -10, 'test': None}, {'idx': 1745227431, 'price': 9, 'quality': 4, 'offer_by': 'buyer', 'stamp': 1745227431, 'from_chat': True, 'enhanced': None, 'profit_bot1': 3, 'profit_bot2': 2, 'test': None}, {'idx': 1745227454, 'price': 6, 'quality': 0, 'offer_by': 'supplier', 'stamp': 1745227454, 'from_chat': True, 'enhanced': None, 'profit_bot1': 2, 'profit_bot2': 3, 'test': None}]</t>
   </si>
 </sst>
 </file>
@@ -2296,10 +2305,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R204"/>
+  <dimension ref="A1:R205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2327,10 +2337,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
@@ -13126,6 +13136,59 @@
       </c>
       <c r="Q204">
         <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>632</v>
+      </c>
+      <c r="B205" t="s">
+        <v>222</v>
+      </c>
+      <c r="C205" t="s">
+        <v>221</v>
+      </c>
+      <c r="D205">
+        <v>8</v>
+      </c>
+      <c r="E205">
+        <v>3</v>
+      </c>
+      <c r="F205">
+        <v>6</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>8</v>
+      </c>
+      <c r="I205">
+        <v>3</v>
+      </c>
+      <c r="J205">
+        <v>2</v>
+      </c>
+      <c r="K205">
+        <v>3</v>
+      </c>
+      <c r="L205">
+        <v>3</v>
+      </c>
+      <c r="M205">
+        <v>9</v>
+      </c>
+      <c r="N205" t="s">
+        <v>633</v>
+      </c>
+      <c r="O205" t="s">
+        <v>634</v>
+      </c>
+      <c r="P205" t="s">
+        <v>631</v>
+      </c>
+      <c r="Q205">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>